<commit_message>
Used SAPFLUXNET data to create predictions, started Penman-Monteith comparison
</commit_message>
<xml_diff>
--- a/data/species_types.xlsx
+++ b/data/species_types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{84A15B6E-34DA-4DDE-8696-C95FC7ACA1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CE48AD95-903F-4409-A089-70A250FEA8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="2310" yWindow="1500" windowWidth="21570" windowHeight="12735"/>
   </bookViews>
   <sheets>
     <sheet name="species_types" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,13 @@
     <t>Count</t>
   </si>
   <si>
-    <t>cold deciduous</t>
-  </si>
-  <si>
     <t>evergreen</t>
   </si>
   <si>
-    <t>drought deciduous</t>
+    <t>deciduous</t>
+  </si>
+  <si>
+    <t>missing</t>
   </si>
 </sst>
 </file>
@@ -590,6 +590,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Species</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Functional Types</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -627,15 +657,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Species Types</c:v>
-          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -644,13 +679,21 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B781-448C-AD2C-30FE67489741}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
@@ -659,21 +702,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-B781-448C-AD2C-30FE67489741}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -690,7 +723,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -707,9 +740,9 @@
             </c:txPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
-            <c:showCatName val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
@@ -732,42 +765,36 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>species_types!$A$2:$A$4</c:f>
+              <c:f>species_types!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>cold deciduous</c:v>
+                  <c:v>evergreen</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>evergreen</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>drought deciduous</c:v>
+                  <c:v>deciduous</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>species_types!$B$2:$B$4</c:f>
+              <c:f>species_types!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-26F6-45C4-B90F-26012E49A448}"/>
+              <c16:uniqueId val="{00000000-B781-448C-AD2C-30FE67489741}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -790,6 +817,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1397,23 +1455,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A004940-E04B-4FD5-BAB7-04EC96756EA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E4B56A-62D8-4A42-B94D-237D50BAA262}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1734,12 +1792,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1760,7 +1818,8 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <f>19+B4</f>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved data files to separate folder to save space on github
</commit_message>
<xml_diff>
--- a/data/species_types.xlsx
+++ b/data/species_types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morga\GitHub\Transpiration-ML-Project\Transpiration-ML-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E995E6-85D0-4BD2-91CF-D55810E8922A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0732E28-579A-4FFD-B213-EE5166159335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1830" windowWidth="21015" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_types" sheetId="1" r:id="rId1"/>
@@ -690,6 +690,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-0A34-4DFA-9605-917BAF75431C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1862,7 +1867,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>